<commit_message>
generalize from pask, add documentation, exception handling
</commit_message>
<xml_diff>
--- a/templates/hämtlista_template.xlsx
+++ b/templates/hämtlista_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\Jupyter\Enterprise\SvenskaKyrkan\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atw10wp4\JupyterLab\Kyrkan\WebShopReport\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5905D7-8D9A-447A-9E28-92EB0570C086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BAF555-AF46-49CE-8EFE-7681E56DB367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Hämtningar</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Datum och tid</t>
-  </si>
-  <si>
-    <t>Påskmarknad 2022</t>
   </si>
 </sst>
 </file>
@@ -534,24 +531,22 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="3.44140625" customWidth="1"/>
+    <col min="1" max="2" width="3.453125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.36328125" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" customWidth="1"/>
+    <col min="8" max="8" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
+    <row r="1" spans="1:9" ht="9.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="13" t="s">
@@ -564,10 +559,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="16"/>
       <c r="C4" s="1" t="s">
         <v>1</v>
@@ -585,7 +580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="11"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17">
@@ -593,7 +588,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="15">
         <v>1</v>
       </c>
@@ -604,7 +599,7 @@
       <c r="G6" s="5"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -613,7 +608,7 @@
       <c r="G7" s="4"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
         <v>4</v>
       </c>

</xml_diff>